<commit_message>
Finished the design of the 1MHz filter
</commit_message>
<xml_diff>
--- a/Docs and papers/Ferr-Inductor_Calc.xlsx
+++ b/Docs and papers/Ferr-Inductor_Calc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AntovI\Desktop\Uni\DR\Docs and papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0108D3CC-554B-4007-BAF0-B474172ED25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BD80AD-B24A-4A84-A3A3-35D3A4BC656A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-90" windowWidth="23280" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28575" yWindow="285" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -249,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -295,9 +295,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -583,7 +580,7 @@
   <dimension ref="B2:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,16 +641,16 @@
       <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
       <c r="E5" s="7">
         <v>3.325E-4</v>
       </c>
       <c r="F5" s="7">
         <v>6.7299999999999996E-5</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
@@ -819,13 +816,13 @@
         <v>0.5</v>
       </c>
       <c r="D12" s="12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E12" s="12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F12" s="12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G12" s="12">
         <v>0.33</v>
@@ -844,15 +841,15 @@
       </c>
       <c r="D13" s="13">
         <f>D10/D12/D12</f>
-        <v>137.74104683195591</v>
+        <v>60</v>
       </c>
       <c r="E13" s="13">
         <f t="shared" ref="E13:H13" si="6">E10/E12/E12</f>
-        <v>137.74104683195591</v>
+        <v>60</v>
       </c>
       <c r="F13" s="13">
         <f t="shared" si="6"/>
-        <v>137.74104683195591</v>
+        <v>60</v>
       </c>
       <c r="G13" s="13">
         <f t="shared" si="6"/>

</xml_diff>